<commit_message>
Changed the file upload method for cloud compatability as well as fixing some commenting errors
</commit_message>
<xml_diff>
--- a/testSheets/testSheet.xlsx
+++ b/testSheets/testSheet.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\max max\Desktop\TTP-Sanitizer\testSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60634C4-E8FC-4DBF-AD3D-62E7E4A18435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1766AAB3-9849-47F8-A5C9-D4448C11FD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PRECEPTORS" sheetId="1" r:id="rId1"/>
+    <sheet name="Preceptor Schedule" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1098,137 +1098,137 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5068,7 +5068,7 @@
   <dimension ref="A1:E196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -5080,32 +5080,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="53"/>
-      <c r="B3" s="53"/>
+      <c r="A3" s="81"/>
+      <c r="B3" s="81"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="53"/>
-      <c r="B4" s="53"/>
+      <c r="A4" s="81"/>
+      <c r="B4" s="81"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="53"/>
-      <c r="B5" s="53"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="81"/>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
@@ -5114,8 +5114,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="53"/>
-      <c r="B6" s="53"/>
+      <c r="A6" s="81"/>
+      <c r="B6" s="81"/>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
@@ -5124,8 +5124,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="53"/>
-      <c r="B7" s="53"/>
+      <c r="A7" s="81"/>
+      <c r="B7" s="81"/>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
@@ -5134,8 +5134,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="53"/>
-      <c r="B8" s="53"/>
+      <c r="A8" s="81"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
@@ -5144,8 +5144,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="53"/>
-      <c r="B9" s="53"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
@@ -5154,8 +5154,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="53"/>
-      <c r="B10" s="53"/>
+      <c r="A10" s="81"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
@@ -5164,8 +5164,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="53"/>
-      <c r="B11" s="53"/>
+      <c r="A11" s="81"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
@@ -5174,45 +5174,45 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="53"/>
-      <c r="B12" s="53"/>
+      <c r="A12" s="81"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="53"/>
-      <c r="B13" s="53"/>
+      <c r="A13" s="81"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="53"/>
-      <c r="B14" s="53"/>
+      <c r="A14" s="81"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="53"/>
-      <c r="B15" s="53"/>
+      <c r="A15" s="81"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="93"/>
     </row>
     <row r="17" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="57"/>
+      <c r="B17" s="94"/>
       <c r="C17" s="10" t="s">
         <v>20</v>
       </c>
@@ -5224,148 +5224,148 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="58"/>
+      <c r="B18" s="89"/>
       <c r="C18" s="11"/>
       <c r="D18" s="12"/>
       <c r="E18" s="13"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="58"/>
+      <c r="B19" s="89"/>
       <c r="C19" s="14"/>
       <c r="D19" s="15"/>
       <c r="E19" s="16"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="58"/>
+      <c r="B20" s="89"/>
       <c r="C20" s="14"/>
       <c r="D20" s="15"/>
       <c r="E20" s="16"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="64"/>
-      <c r="B21" s="64"/>
+      <c r="A21" s="90"/>
+      <c r="B21" s="90"/>
       <c r="C21" s="17"/>
       <c r="D21" s="18"/>
       <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="53"/>
-      <c r="B22" s="53"/>
+      <c r="A22" s="81"/>
+      <c r="B22" s="81"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="53"/>
-      <c r="B23" s="53"/>
+      <c r="A23" s="81"/>
+      <c r="B23" s="81"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="53"/>
-      <c r="B24" s="53"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="81"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="59" t="s">
+      <c r="A25" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="61"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="88"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="62"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="63"/>
+      <c r="A26" s="80"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="82"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="62"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="63"/>
+      <c r="A27" s="80"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="82"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="62"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="63"/>
+      <c r="A28" s="80"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="82"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="62"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="63"/>
+      <c r="A29" s="80"/>
+      <c r="B29" s="81"/>
+      <c r="C29" s="81"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="82"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="62"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="63"/>
+      <c r="A30" s="80"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="82"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="62"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="63"/>
+      <c r="A31" s="80"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="82"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="75"/>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="77"/>
+      <c r="A32" s="83"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="85"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="53"/>
-      <c r="B33" s="53"/>
+      <c r="A33" s="81"/>
+      <c r="B33" s="81"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="53"/>
-      <c r="B34" s="53"/>
+      <c r="A34" s="81"/>
+      <c r="B34" s="81"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="76"/>
-      <c r="B35" s="76"/>
+      <c r="A35" s="84"/>
+      <c r="B35" s="84"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="78" t="s">
+      <c r="A36" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="79"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="80"/>
-      <c r="E36" s="81"/>
+      <c r="B36" s="77"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="79"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="65" t="s">
+      <c r="A37" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="66"/>
-      <c r="C37" s="66"/>
-      <c r="D37" s="67" t="s">
+      <c r="B37" s="63"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="68"/>
+      <c r="E37" s="65"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="20" t="s">
@@ -5385,10 +5385,10 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="69">
+      <c r="A39" s="52">
         <v>45821</v>
       </c>
-      <c r="B39" s="72" t="s">
+      <c r="B39" s="54" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="24" t="s">
@@ -5402,8 +5402,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="70"/>
-      <c r="B40" s="73"/>
+      <c r="A40" s="75"/>
+      <c r="B40" s="66"/>
       <c r="C40" s="26" t="s">
         <v>68</v>
       </c>
@@ -5415,7 +5415,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="71"/>
+      <c r="A41" s="53"/>
       <c r="B41" s="29" t="s">
         <v>31</v>
       </c>
@@ -5430,10 +5430,10 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="69">
+      <c r="A42" s="52">
         <v>45826</v>
       </c>
-      <c r="B42" s="72" t="s">
+      <c r="B42" s="54" t="s">
         <v>32</v>
       </c>
       <c r="C42" s="24" t="s">
@@ -5447,8 +5447,8 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="71"/>
-      <c r="B43" s="74"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="55"/>
       <c r="C43" s="30" t="s">
         <v>68</v>
       </c>
@@ -5477,10 +5477,10 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="69">
+      <c r="A45" s="52">
         <v>45828</v>
       </c>
-      <c r="B45" s="72" t="s">
+      <c r="B45" s="54" t="s">
         <v>33</v>
       </c>
       <c r="C45" s="24" t="s">
@@ -5494,8 +5494,8 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="70"/>
-      <c r="B46" s="74"/>
+      <c r="A46" s="75"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="30" t="s">
         <v>69</v>
       </c>
@@ -5507,8 +5507,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="70"/>
-      <c r="B47" s="72" t="s">
+      <c r="A47" s="75"/>
+      <c r="B47" s="54" t="s">
         <v>30</v>
       </c>
       <c r="C47" s="24" t="s">
@@ -5522,8 +5522,8 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="70"/>
-      <c r="B48" s="73"/>
+      <c r="A48" s="75"/>
+      <c r="B48" s="66"/>
       <c r="C48" s="26" t="s">
         <v>68</v>
       </c>
@@ -5535,7 +5535,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="71"/>
+      <c r="A49" s="53"/>
       <c r="B49" s="29" t="s">
         <v>34</v>
       </c>
@@ -5567,24 +5567,24 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="78" t="s">
+      <c r="A54" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="B54" s="79"/>
-      <c r="C54" s="79"/>
-      <c r="D54" s="80"/>
-      <c r="E54" s="81"/>
+      <c r="B54" s="77"/>
+      <c r="C54" s="77"/>
+      <c r="D54" s="78"/>
+      <c r="E54" s="79"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="65" t="s">
+      <c r="A55" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="B55" s="66"/>
-      <c r="C55" s="66"/>
-      <c r="D55" s="67" t="s">
+      <c r="B55" s="63"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="E55" s="68"/>
+      <c r="E55" s="65"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="36" t="s">
@@ -5621,7 +5621,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="69">
+      <c r="A58" s="52">
         <v>45820</v>
       </c>
       <c r="B58" s="33" t="s">
@@ -5638,8 +5638,8 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="70"/>
-      <c r="B59" s="72" t="s">
+      <c r="A59" s="75"/>
+      <c r="B59" s="54" t="s">
         <v>32</v>
       </c>
       <c r="C59" s="24" t="s">
@@ -5653,8 +5653,8 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="71"/>
-      <c r="B60" s="74"/>
+      <c r="A60" s="53"/>
+      <c r="B60" s="55"/>
       <c r="C60" s="30" t="s">
         <v>69</v>
       </c>
@@ -5666,10 +5666,10 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="69">
+      <c r="A61" s="52">
         <v>45821</v>
       </c>
-      <c r="B61" s="72" t="s">
+      <c r="B61" s="54" t="s">
         <v>33</v>
       </c>
       <c r="C61" s="24" t="s">
@@ -5683,8 +5683,8 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="71"/>
-      <c r="B62" s="74"/>
+      <c r="A62" s="53"/>
+      <c r="B62" s="55"/>
       <c r="C62" s="30" t="s">
         <v>68</v>
       </c>
@@ -5728,99 +5728,99 @@
       <c r="E66" s="2"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="82" t="s">
+      <c r="A67" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="B67" s="83"/>
-      <c r="C67" s="83"/>
-      <c r="D67" s="83"/>
-      <c r="E67" s="84"/>
+      <c r="B67" s="69"/>
+      <c r="C67" s="69"/>
+      <c r="D67" s="69"/>
+      <c r="E67" s="70"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="65" t="s">
+      <c r="A68" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="B68" s="66"/>
-      <c r="C68" s="66"/>
-      <c r="D68" s="67" t="s">
+      <c r="B68" s="63"/>
+      <c r="C68" s="63"/>
+      <c r="D68" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="E68" s="68"/>
+      <c r="E68" s="65"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="65" t="s">
+      <c r="A69" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="B69" s="66"/>
-      <c r="C69" s="66"/>
-      <c r="D69" s="67" t="s">
+      <c r="B69" s="63"/>
+      <c r="C69" s="63"/>
+      <c r="D69" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="E69" s="68"/>
+      <c r="E69" s="65"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="65" t="s">
+      <c r="A70" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="B70" s="66"/>
-      <c r="C70" s="66"/>
-      <c r="D70" s="67" t="s">
+      <c r="B70" s="63"/>
+      <c r="C70" s="63"/>
+      <c r="D70" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="E70" s="68"/>
+      <c r="E70" s="65"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="65" t="s">
+      <c r="A71" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="B71" s="66"/>
-      <c r="C71" s="66"/>
-      <c r="D71" s="67" t="s">
+      <c r="B71" s="63"/>
+      <c r="C71" s="63"/>
+      <c r="D71" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="E71" s="68"/>
+      <c r="E71" s="65"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="65" t="s">
+      <c r="A72" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="66"/>
-      <c r="C72" s="66"/>
-      <c r="D72" s="67" t="s">
+      <c r="B72" s="63"/>
+      <c r="C72" s="63"/>
+      <c r="D72" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="E72" s="68"/>
+      <c r="E72" s="65"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="65" t="s">
+      <c r="A73" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="B73" s="66"/>
-      <c r="C73" s="66"/>
-      <c r="D73" s="67" t="s">
+      <c r="B73" s="63"/>
+      <c r="C73" s="63"/>
+      <c r="D73" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="E73" s="68"/>
+      <c r="E73" s="65"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="82" t="s">
+      <c r="A74" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="B74" s="83"/>
-      <c r="C74" s="83"/>
-      <c r="D74" s="83"/>
-      <c r="E74" s="84"/>
+      <c r="B74" s="69"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="69"/>
+      <c r="E74" s="70"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="85" t="s">
+      <c r="A75" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="B75" s="86"/>
-      <c r="C75" s="86"/>
-      <c r="D75" s="87" t="s">
+      <c r="B75" s="72"/>
+      <c r="C75" s="72"/>
+      <c r="D75" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="E75" s="88"/>
+      <c r="E75" s="74"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="20" t="s">
@@ -5982,15 +5982,15 @@
       <c r="E88" s="43"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="89" t="s">
+      <c r="A89" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="B89" s="90"/>
-      <c r="C89" s="90"/>
-      <c r="D89" s="91" t="s">
+      <c r="B89" s="59"/>
+      <c r="C89" s="59"/>
+      <c r="D89" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="E89" s="92"/>
+      <c r="E89" s="61"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="45" t="s">
@@ -6065,15 +6065,15 @@
       <c r="E95" s="48"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" s="89" t="s">
+      <c r="A96" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="B96" s="90"/>
-      <c r="C96" s="90"/>
-      <c r="D96" s="91" t="s">
+      <c r="B96" s="59"/>
+      <c r="C96" s="59"/>
+      <c r="D96" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="E96" s="92"/>
+      <c r="E96" s="61"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="45" t="s">
@@ -6093,30 +6093,30 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A98" s="69">
+      <c r="A98" s="52">
         <v>45824</v>
       </c>
       <c r="B98" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C98" s="72" t="s">
+      <c r="C98" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="D98" s="72" t="s">
+      <c r="D98" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="E98" s="93" t="s">
+      <c r="E98" s="56" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A99" s="71"/>
+      <c r="A99" s="53"/>
       <c r="B99" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C99" s="74"/>
-      <c r="D99" s="74"/>
-      <c r="E99" s="94"/>
+      <c r="C99" s="55"/>
+      <c r="D99" s="55"/>
+      <c r="E99" s="57"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="34" t="s">
@@ -6157,15 +6157,15 @@
       <c r="E103" s="48"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A104" s="89" t="s">
+      <c r="A104" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="B104" s="90"/>
-      <c r="C104" s="90"/>
-      <c r="D104" s="91" t="s">
+      <c r="B104" s="59"/>
+      <c r="C104" s="59"/>
+      <c r="D104" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="E104" s="92"/>
+      <c r="E104" s="61"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="45" t="s">
@@ -6240,15 +6240,15 @@
       <c r="E110" s="48"/>
     </row>
     <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="95" t="s">
+      <c r="A111" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="B111" s="90"/>
-      <c r="C111" s="90"/>
-      <c r="D111" s="91" t="s">
+      <c r="B111" s="59"/>
+      <c r="C111" s="59"/>
+      <c r="D111" s="60" t="s">
         <v>114</v>
       </c>
-      <c r="E111" s="92"/>
+      <c r="E111" s="61"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="45" t="s">
@@ -6268,30 +6268,30 @@
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A113" s="69">
+      <c r="A113" s="52">
         <v>45825</v>
       </c>
       <c r="B113" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C113" s="72" t="s">
+      <c r="C113" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="D113" s="72" t="s">
+      <c r="D113" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="E113" s="93" t="s">
+      <c r="E113" s="56" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A114" s="71"/>
+      <c r="A114" s="53"/>
       <c r="B114" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C114" s="74"/>
-      <c r="D114" s="74"/>
-      <c r="E114" s="94"/>
+      <c r="C114" s="55"/>
+      <c r="D114" s="55"/>
+      <c r="E114" s="57"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="34" t="s">
@@ -6332,15 +6332,15 @@
       <c r="E118" s="48"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A119" s="89" t="s">
+      <c r="A119" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="B119" s="90"/>
-      <c r="C119" s="90"/>
-      <c r="D119" s="91" t="s">
+      <c r="B119" s="59"/>
+      <c r="C119" s="59"/>
+      <c r="D119" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="E119" s="92"/>
+      <c r="E119" s="61"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="45" t="s">
@@ -6363,16 +6363,16 @@
       <c r="A121" s="38">
         <v>45819</v>
       </c>
-      <c r="B121" s="72" t="s">
+      <c r="B121" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C121" s="72" t="s">
+      <c r="C121" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="D121" s="72" t="s">
+      <c r="D121" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="E121" s="93" t="s">
+      <c r="E121" s="56" t="s">
         <v>117</v>
       </c>
     </row>
@@ -6380,10 +6380,10 @@
       <c r="A122" s="38">
         <v>45820</v>
       </c>
-      <c r="B122" s="74"/>
-      <c r="C122" s="74"/>
-      <c r="D122" s="74"/>
-      <c r="E122" s="94"/>
+      <c r="B122" s="55"/>
+      <c r="C122" s="55"/>
+      <c r="D122" s="55"/>
+      <c r="E122" s="57"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="34" t="s">
@@ -6424,15 +6424,15 @@
       <c r="E126" s="43"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A127" s="65" t="s">
+      <c r="A127" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="B127" s="66"/>
-      <c r="C127" s="66"/>
-      <c r="D127" s="67" t="s">
+      <c r="B127" s="63"/>
+      <c r="C127" s="63"/>
+      <c r="D127" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="E127" s="68"/>
+      <c r="E127" s="65"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="45" t="s">
@@ -6507,15 +6507,15 @@
       <c r="E133" s="43"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A134" s="65" t="s">
+      <c r="A134" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="B134" s="66"/>
-      <c r="C134" s="66"/>
-      <c r="D134" s="67" t="s">
+      <c r="B134" s="63"/>
+      <c r="C134" s="63"/>
+      <c r="D134" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="E134" s="68"/>
+      <c r="E134" s="65"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="45" t="s">
@@ -6538,7 +6538,7 @@
       <c r="A136" s="38">
         <v>45825</v>
       </c>
-      <c r="B136" s="72" t="s">
+      <c r="B136" s="54" t="s">
         <v>44</v>
       </c>
       <c r="C136" s="24" t="s">
@@ -6555,7 +6555,7 @@
       <c r="A137" s="38">
         <v>45827</v>
       </c>
-      <c r="B137" s="73"/>
+      <c r="B137" s="66"/>
       <c r="C137" s="26" t="s">
         <v>69</v>
       </c>
@@ -6570,7 +6570,7 @@
       <c r="A138" s="28">
         <v>45828</v>
       </c>
-      <c r="B138" s="74"/>
+      <c r="B138" s="55"/>
       <c r="C138" s="30" t="s">
         <v>68</v>
       </c>
@@ -6620,15 +6620,15 @@
       <c r="E142" s="43"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A143" s="89" t="s">
+      <c r="A143" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="B143" s="90"/>
-      <c r="C143" s="90"/>
-      <c r="D143" s="91" t="s">
+      <c r="B143" s="59"/>
+      <c r="C143" s="59"/>
+      <c r="D143" s="60" t="s">
         <v>115</v>
       </c>
-      <c r="E143" s="92"/>
+      <c r="E143" s="61"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="45" t="s">
@@ -6703,15 +6703,15 @@
       <c r="E149" s="43"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A150" s="89" t="s">
+      <c r="A150" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="B150" s="90"/>
-      <c r="C150" s="90"/>
-      <c r="D150" s="91" t="s">
+      <c r="B150" s="59"/>
+      <c r="C150" s="59"/>
+      <c r="D150" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="E150" s="92"/>
+      <c r="E150" s="61"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="45" t="s">
@@ -6786,15 +6786,15 @@
       <c r="E156" s="43"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A157" s="89" t="s">
+      <c r="A157" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="B157" s="90"/>
-      <c r="C157" s="90"/>
-      <c r="D157" s="91" t="s">
+      <c r="B157" s="59"/>
+      <c r="C157" s="59"/>
+      <c r="D157" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="E157" s="92"/>
+      <c r="E157" s="61"/>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="45" t="s">
@@ -6817,16 +6817,16 @@
       <c r="A159" s="38">
         <v>45819</v>
       </c>
-      <c r="B159" s="72" t="s">
+      <c r="B159" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C159" s="72" t="s">
+      <c r="C159" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="D159" s="72" t="s">
+      <c r="D159" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="E159" s="93" t="s">
+      <c r="E159" s="56" t="s">
         <v>116</v>
       </c>
     </row>
@@ -6834,10 +6834,10 @@
       <c r="A160" s="38">
         <v>45826</v>
       </c>
-      <c r="B160" s="74"/>
-      <c r="C160" s="74"/>
-      <c r="D160" s="74"/>
-      <c r="E160" s="94"/>
+      <c r="B160" s="55"/>
+      <c r="C160" s="55"/>
+      <c r="D160" s="55"/>
+      <c r="E160" s="57"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="34" t="s">
@@ -6878,15 +6878,15 @@
       <c r="E164" s="43"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A165" s="89" t="s">
+      <c r="A165" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="B165" s="90"/>
-      <c r="C165" s="90"/>
-      <c r="D165" s="91" t="s">
+      <c r="B165" s="59"/>
+      <c r="C165" s="59"/>
+      <c r="D165" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="E165" s="92"/>
+      <c r="E165" s="61"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="45" t="s">
@@ -6906,30 +6906,30 @@
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A167" s="69">
+      <c r="A167" s="52">
         <v>45824</v>
       </c>
       <c r="B167" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C167" s="72" t="s">
+      <c r="C167" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="D167" s="72" t="s">
+      <c r="D167" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="E167" s="93" t="s">
+      <c r="E167" s="56" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A168" s="71"/>
+      <c r="A168" s="53"/>
       <c r="B168" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C168" s="74"/>
-      <c r="D168" s="74"/>
-      <c r="E168" s="94"/>
+      <c r="C168" s="55"/>
+      <c r="D168" s="55"/>
+      <c r="E168" s="57"/>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="34" t="s">
@@ -6970,15 +6970,15 @@
       <c r="E172" s="48"/>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A173" s="89" t="s">
+      <c r="A173" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="B173" s="90"/>
-      <c r="C173" s="90"/>
-      <c r="D173" s="91" t="s">
+      <c r="B173" s="59"/>
+      <c r="C173" s="59"/>
+      <c r="D173" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="E173" s="92"/>
+      <c r="E173" s="61"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="45" t="s">
@@ -7087,15 +7087,15 @@
       <c r="E181" s="48"/>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A182" s="89" t="s">
+      <c r="A182" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="B182" s="90"/>
-      <c r="C182" s="90"/>
-      <c r="D182" s="91" t="s">
+      <c r="B182" s="59"/>
+      <c r="C182" s="59"/>
+      <c r="D182" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="E182" s="92"/>
+      <c r="E182" s="61"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="45" t="s">
@@ -7118,7 +7118,7 @@
       <c r="A184" s="38">
         <v>45825</v>
       </c>
-      <c r="B184" s="72" t="s">
+      <c r="B184" s="54" t="s">
         <v>64</v>
       </c>
       <c r="C184" s="39" t="s">
@@ -7135,7 +7135,7 @@
       <c r="A185" s="38">
         <v>45826</v>
       </c>
-      <c r="B185" s="74"/>
+      <c r="B185" s="55"/>
       <c r="C185" s="39" t="s">
         <v>69</v>
       </c>
@@ -7185,15 +7185,15 @@
       <c r="E189" s="43"/>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A190" s="65" t="s">
+      <c r="A190" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="B190" s="66"/>
-      <c r="C190" s="66"/>
-      <c r="D190" s="67" t="s">
+      <c r="B190" s="63"/>
+      <c r="C190" s="63"/>
+      <c r="D190" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="E190" s="68"/>
+      <c r="E190" s="65"/>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="20" t="s">
@@ -7213,30 +7213,30 @@
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A192" s="69">
+      <c r="A192" s="52">
         <v>45818</v>
       </c>
       <c r="B192" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C192" s="72" t="s">
+      <c r="C192" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="D192" s="72" t="s">
+      <c r="D192" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="E192" s="93" t="s">
+      <c r="E192" s="56" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A193" s="71"/>
+      <c r="A193" s="53"/>
       <c r="B193" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C193" s="74"/>
-      <c r="D193" s="74"/>
-      <c r="E193" s="94"/>
+      <c r="C193" s="55"/>
+      <c r="D193" s="55"/>
+      <c r="E193" s="57"/>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="34" t="s">
@@ -7271,44 +7271,76 @@
     </row>
   </sheetData>
   <mergeCells count="124">
-    <mergeCell ref="A192:A193"/>
-    <mergeCell ref="C192:C193"/>
-    <mergeCell ref="D192:D193"/>
-    <mergeCell ref="E192:E193"/>
-    <mergeCell ref="A173:C173"/>
-    <mergeCell ref="D173:E173"/>
-    <mergeCell ref="A182:C182"/>
-    <mergeCell ref="D182:E182"/>
-    <mergeCell ref="B184:B185"/>
-    <mergeCell ref="A190:C190"/>
-    <mergeCell ref="D190:E190"/>
-    <mergeCell ref="A165:C165"/>
-    <mergeCell ref="D165:E165"/>
-    <mergeCell ref="A167:A168"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="D167:D168"/>
-    <mergeCell ref="E167:E168"/>
-    <mergeCell ref="A150:C150"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="A157:C157"/>
-    <mergeCell ref="D157:E157"/>
-    <mergeCell ref="B159:B160"/>
-    <mergeCell ref="C159:C160"/>
-    <mergeCell ref="D159:D160"/>
-    <mergeCell ref="E159:E160"/>
-    <mergeCell ref="A127:C127"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="A134:C134"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="B136:B138"/>
-    <mergeCell ref="A143:C143"/>
-    <mergeCell ref="D143:E143"/>
-    <mergeCell ref="A119:C119"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="B121:B122"/>
-    <mergeCell ref="C121:C122"/>
-    <mergeCell ref="D121:D122"/>
-    <mergeCell ref="E121:E122"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="A74:E74"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="D71:E71"/>
     <mergeCell ref="A104:C104"/>
     <mergeCell ref="D104:E104"/>
     <mergeCell ref="A111:C111"/>
@@ -7325,76 +7357,44 @@
     <mergeCell ref="D98:D99"/>
     <mergeCell ref="E98:E99"/>
     <mergeCell ref="C113:C114"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="A74:E74"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="A67:E67"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A127:C127"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="A134:C134"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="B136:B138"/>
+    <mergeCell ref="A143:C143"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="A119:C119"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="B121:B122"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="D121:D122"/>
+    <mergeCell ref="E121:E122"/>
+    <mergeCell ref="A165:C165"/>
+    <mergeCell ref="D165:E165"/>
+    <mergeCell ref="A167:A168"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="D167:D168"/>
+    <mergeCell ref="E167:E168"/>
+    <mergeCell ref="A150:C150"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="A157:C157"/>
+    <mergeCell ref="D157:E157"/>
+    <mergeCell ref="B159:B160"/>
+    <mergeCell ref="C159:C160"/>
+    <mergeCell ref="D159:D160"/>
+    <mergeCell ref="E159:E160"/>
+    <mergeCell ref="A192:A193"/>
+    <mergeCell ref="C192:C193"/>
+    <mergeCell ref="D192:D193"/>
+    <mergeCell ref="E192:E193"/>
+    <mergeCell ref="A173:C173"/>
+    <mergeCell ref="D173:E173"/>
+    <mergeCell ref="A182:C182"/>
+    <mergeCell ref="D182:E182"/>
+    <mergeCell ref="B184:B185"/>
+    <mergeCell ref="A190:C190"/>
+    <mergeCell ref="D190:E190"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>